<commit_message>
Fix pay period 26 hours precision and equity/paid split
- Fix Ariful hours from 66.00 to 66.50 (was missing 0.5h meeting entry)
- Use v2.csv export which correctly includes all 160 timesheet entries
- Update metadata to point to v2 as latest (v3 had incomplete export)
- Add equity/paid hours split to users.json (equity filled first, paid capped)
- Update HoursReportGenerator to calculate equity-first allocation
- Fix KimaiExporter URL encoding for date range filter
- Regenerate all reports and pay period CSV/XLSX with correct values
- Total expense updated from $3,860 to $3,865
</commit_message>
<xml_diff>
--- a/kimai-data/26/pay-period-26.xlsx
+++ b/kimai-data/26/pay-period-26.xlsx
@@ -477,12 +477,9 @@
         <f>F6 + G6</f>
       </c>
       <c r="F6">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="G6">
-        <v>40</v>
-      </c>
-      <c r="H6">
         <v>40</v>
       </c>
       <c r="I6" t="str">
@@ -506,13 +503,10 @@
         <f>F7 + G7</f>
       </c>
       <c r="F7">
-        <v>66.5</v>
+        <v>26.5</v>
       </c>
       <c r="G7">
-        <v>33.25</v>
-      </c>
-      <c r="H7">
-        <v>33.25</v>
+        <v>40</v>
       </c>
       <c r="I7" t="str">
         <v>Short 13.50 hours</v>
@@ -535,13 +529,10 @@
         <f>F8 + G8</f>
       </c>
       <c r="F8">
-        <v>87.5</v>
+        <v>40</v>
       </c>
       <c r="G8">
-        <v>43.75</v>
-      </c>
-      <c r="H8">
-        <v>43.75</v>
+        <v>40</v>
       </c>
       <c r="I8" t="str">
         <v>Extra 7.50 hours carry over</v>
@@ -564,12 +555,9 @@
         <f>F9 + G9</f>
       </c>
       <c r="F9">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="G9">
-        <v>40</v>
-      </c>
-      <c r="H9">
         <v>40</v>
       </c>
       <c r="I9" t="str">
@@ -593,12 +581,9 @@
         <f>F10 + G10</f>
       </c>
       <c r="F10">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="G10">
-        <v>10</v>
-      </c>
-      <c r="H10">
         <v>40</v>
       </c>
       <c r="I10" t="str">
@@ -622,13 +607,10 @@
         <f>F11 + G11</f>
       </c>
       <c r="F11">
-        <v>84.83333333333333</v>
+        <v>40</v>
       </c>
       <c r="G11">
-        <v>42.416666666666664</v>
-      </c>
-      <c r="H11">
-        <v>42.416666666666664</v>
+        <v>40</v>
       </c>
       <c r="I11" t="str">
         <v>Extra 4.83 hours carry over</v>
@@ -651,16 +633,13 @@
         <f>F12 + G12</f>
       </c>
       <c r="F12">
-        <v>56</v>
-      </c>
-      <c r="G12" t="str">
-        <v/>
-      </c>
-      <c r="H12">
-        <v>56</v>
+        <v>5</v>
+      </c>
+      <c r="G12">
+        <v>40</v>
       </c>
       <c r="I12" t="str">
-        <v>Extra 16.00 hours carry over</v>
+        <v>Extra 11.00 hours carry over</v>
       </c>
     </row>
     <row r="13">
@@ -680,16 +659,13 @@
         <f>F13 + G13</f>
       </c>
       <c r="F13">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="G13">
-        <v>40</v>
-      </c>
-      <c r="H13">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="I13" t="str">
-        <v/>
+        <v>Short 20.00 hours</v>
       </c>
     </row>
     <row r="14">
@@ -932,13 +908,13 @@
         <v>Edward Obi</v>
       </c>
       <c r="B22">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C22">
         <f>C22 * 2</f>
       </c>
       <c r="D22">
-        <v>20</v>
+        <v>22.5</v>
       </c>
       <c r="E22">
         <f>ROUND(F22 * J22, 2)</f>
@@ -970,7 +946,7 @@
         <f>C23 * 2</f>
       </c>
       <c r="D23">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E23">
         <f>ROUND(F23 * J23, 2)</f>
@@ -1002,7 +978,7 @@
         <v>3 hour+ difference</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E24">
         <f>ROUND(F24 * J24, 2)</f>
@@ -1011,7 +987,7 @@
         <f>ROUND(G24 * H24 * I24, 2)</f>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H24">
         <v>1</v>
@@ -1048,6 +1024,12 @@
       <c r="H25" t="str">
         <v>Total Expected Paid Weekly Hours (C)</v>
       </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
@@ -1274,7 +1256,7 @@
         <f>G34 + H34</f>
       </c>
       <c r="G34">
-        <v>20</v>
+        <v>22.5</v>
       </c>
       <c r="H34">
         <f>D22</f>
@@ -1282,7 +1264,7 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>Forrest</v>
+        <v>Dennis Fisher</v>
       </c>
       <c r="B35">
         <f>IF(C35 &gt; 0, TEXT(C35 / E35 * 100, "0.00") &amp; "% Missed", IF(C35 &lt; 0, TEXT(-C35 / E35 * 100, "0.00") &amp; "% Overworked", "No Difference"))</f>
@@ -1300,7 +1282,7 @@
         <f>G35 + H35</f>
       </c>
       <c r="G35">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="H35">
         <f>D23</f>
@@ -1308,7 +1290,7 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>Dennis</v>
+        <v>Forrest Cordova</v>
       </c>
       <c r="B36">
         <f>IF(C36 &gt; 0, TEXT(C36 / E36 * 100, "0.00") &amp; "% Missed", IF(C36 &lt; 0, TEXT(-C36 / E36 * 100, "0.00") &amp; "% Overworked", "No Difference"))</f>
@@ -1326,7 +1308,7 @@
         <f>G36 + H36</f>
       </c>
       <c r="G36">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H36">
         <f>D24</f>

</xml_diff>